<commit_message>
Integrated API with frontend
</commit_message>
<xml_diff>
--- a/backend/routes/training_set.xlsx
+++ b/backend/routes/training_set.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a769a88f1f7a71a/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38C1B701-7BFD-42DB-B0E6-45DF69ED26D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BD555A-A3C7-4302-AE5B-96F16A9DE6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="127">
   <si>
     <t>Questions</t>
   </si>
@@ -57,21 +57,12 @@
     <t>Are there any additional exams or assessments required for admissions?</t>
   </si>
   <si>
-    <t>What is the cutoff score for MHT-CET and JEE for Computer Science?</t>
-  </si>
-  <si>
-    <t>What is the cutoff score for MHT-CET and JEE for AIDS?</t>
-  </si>
-  <si>
     <t>What is the cutoff score for MHT-CET and JEE for EnTC?</t>
   </si>
   <si>
     <t>What is the cutoff score for MHT-CET and JEE for Civil?</t>
   </si>
   <si>
-    <t>What is the cutoff score for MHT-CET and JEE for IT?</t>
-  </si>
-  <si>
     <t>Are there any reservation criteria for admissions through JEE Main?</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>What is the process for changing my program preference after admission?</t>
   </si>
   <si>
-    <t>What are the accommodation options available for admitted students?</t>
-  </si>
-  <si>
     <t>Can I apply for on-campus housing after being admitted?</t>
   </si>
   <si>
@@ -285,19 +273,31 @@
     <t>Yes, we conduct study abroad programs.</t>
   </si>
   <si>
-    <t>What is the intake of B.Tech Computer Science?</t>
-  </si>
-  <si>
     <t>We currently have an intake of 240 students for this program</t>
   </si>
   <si>
-    <t>What is the intake of B.Tech Information Technology?</t>
-  </si>
-  <si>
     <t>We currently have an intake of 180 students for this program</t>
   </si>
   <si>
-    <t>What is the intake of B.Tech CS?</t>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>What is the cutoff score for MHT-CET and JEE for IT(Information Technology)?</t>
+  </si>
+  <si>
+    <t>What is the cutoff score for MHT-CET and JEE for CS(Computer Science)?</t>
+  </si>
+  <si>
+    <t>Where is the college located?</t>
+  </si>
+  <si>
+    <t>VIIT is located in Kondhwa</t>
+  </si>
+  <si>
+    <t>What is the intake of B.Tech IT(Information Technology)?</t>
+  </si>
+  <si>
+    <t>What is the intake of B.Tech CS(Computer Science)?</t>
   </si>
   <si>
     <t>Where can I find the syllabus for my course?</t>
@@ -309,15 +309,15 @@
     <t>What are some campus dining options?</t>
   </si>
   <si>
+    <t>We have a variety of canteen in campus none of which you'll like but you have to eat it.</t>
+  </si>
+  <si>
+    <t>Hi,Hello,Hola</t>
+  </si>
+  <si>
     <t>Hello! 😊 How can I assist you today? If you have any questions or need information, feel free to ask.</t>
   </si>
   <si>
-    <t>We have a variety of canteen in campus none of which you'll like but you have to eat it.</t>
-  </si>
-  <si>
-    <t>Hi,Hello,Hola</t>
-  </si>
-  <si>
     <t>How can I join a student club or organization?</t>
   </si>
   <si>
@@ -360,9 +360,6 @@
     <t xml:space="preserve">For that issue you can contact our accout's person at xxxxxxxxxx. </t>
   </si>
   <si>
-    <t>How can I select the open elective subject.</t>
-  </si>
-  <si>
     <t>You'll se a dropdown just below your subjects at ht epage you are doing subject registration there you can select the particular elective of your choice.</t>
   </si>
   <si>
@@ -370,6 +367,45 @@
   </si>
   <si>
     <t>Sorry for the inconvinience.The seat's of the particular subject you want might've been totally filled.</t>
+  </si>
+  <si>
+    <t>What is the cutoff score for MHT-CET and JEE for AIDS(Arificial Intelligence and Data Science)?</t>
+  </si>
+  <si>
+    <t>How can I select the open elective subject?</t>
+  </si>
+  <si>
+    <t>How to do Subject Registration?</t>
+  </si>
+  <si>
+    <t>Login into your VIERP account and there you can do the subject registration.</t>
+  </si>
+  <si>
+    <t>IT(Information Technology) cutoff?</t>
+  </si>
+  <si>
+    <t>CS(Computer Science) cutoff?</t>
+  </si>
+  <si>
+    <t>IT(Information Technology) intake?</t>
+  </si>
+  <si>
+    <t>CS(Computer Science) intake?</t>
+  </si>
+  <si>
+    <t>Location of College</t>
+  </si>
+  <si>
+    <t>Name of College</t>
+  </si>
+  <si>
+    <t>Vishwakarma Institute of Information Technology(VIIT). It is located in Kondhwa.</t>
+  </si>
+  <si>
+    <t>What are the accommodation/hostel options available for admitted students?</t>
+  </si>
+  <si>
+    <t>What are the hostel facilities available for admitted students?</t>
   </si>
 </sst>
 </file>
@@ -711,405 +747,540 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="90.109375" customWidth="1"/>
-    <col min="2" max="2" width="116.5546875" customWidth="1"/>
+    <col min="1" max="1" width="96.44140625" customWidth="1"/>
+    <col min="2" max="2" width="97.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B26" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B27" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B28" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B29" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="C29" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B31" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B32" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B33" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="B34" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C34" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="B35" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
+      <c r="C35" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
+      <c r="C36" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A36" s="4" t="s">
+      <c r="C37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A37" s="4" t="s">
+      <c r="C38" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
+      <c r="C39" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
+      <c r="C40" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
+      <c r="C41" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+      <c r="C42" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A43" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
+      <c r="C43" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A44" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    </row>
+    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>96</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>94</v>
@@ -1117,78 +1288,144 @@
     </row>
     <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>114</v>
+    </row>
+    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>